<commit_message>
Get daily reddit data: Tue Jun 25 08:10:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_30.xlsx
+++ b/data/2024_06_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C483"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3100 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1do0cdp</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>I've won the battle to get a nude instead of anything else</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do0cdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1dnzs3e</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Got my nails done in Vietnam</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnzs3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1dnzrtm</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23b45ltq1o8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1dnzqpx</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Learning builder gel extensions - just did a set I'm super proud of! </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkxpechd1o8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1dnzl8d</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Beautiful design by me</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tco0f1l9zn8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1dnzexx</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My client loved her nails 💅  </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnzexx</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1dnzdl3</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Pride dots!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqn6q96uwn8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1dnynhz</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnynhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1dnylde</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Last week of pride nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnylde</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1dnyhx4</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Seria Nail Stickers 🧸🍓</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnyhx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1dny5m7</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Former nail biter… slightly grown out regular nail polish on natural nails 😁</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x08lgpiin8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1dnxei1</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Too pink?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qt2uoeaan8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1dnwytq</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>yes or no?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e39cy16y5n8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1dnww4x</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My team may not have won the Stanley Cup tonight but I still repped them proudly!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnww4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1dnwtkg</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Did I do my orange idiot justice?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnwtkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1dnwnf5</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>No, a 10 yr. old didn't do my nails. Just me, doing my best😺</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnwnf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1dnwilf</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I want my natural nails to grow under acrylics</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnwilf/i_want_my_natural_nails_to_grow_under_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1dnwhvp</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>First time doing BIAB</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpvoxq491n8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1dnvxkf</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Tried to go for a water droplet look 💧</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnvxkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1dnve2v</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnve2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1dnva9f</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time posting nails on reddit </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnva9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1dnv8uz</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today I acquired tiny tiny googley eyes and glow in the dark paints I am excited pictures soon </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnv8uz/today_i_acquired_tiny_tiny_googley_eyes_and_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1dnv790</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Got my nails done, absolutely obsessed 🥹</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vg325smvom8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1dnv6id</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>hit or miss? from a month-old nail tech</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au7pdoqoom8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1dnv1j1</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Is it normal for my nails to be too thin for gel after one gel application and removal?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnv1j1/is_it_normal_for_my_nails_to_be_too_thin_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1dnv1at</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>recent sets</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnv1at</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1dnuz5l</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>I made press ons :)</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnuz5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1dnuvpt</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Bachelorette ready!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om6nvb8ulm8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1dnusv5</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Vacation Nails 🏝️😁</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sunsmds4lm8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1dnuqh2</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Best primer!?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnuqh2/best_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1dnunlm</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Perfect Color</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnunlm</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1dnujp1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Pink Cat-Eye Nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnujp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1dnujfj</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>the difference between my roommates nail/nailbed size and mine 💀</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bjckb2sim8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1dnuj1s</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Blue flower nails to match my wedding dress</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnuj1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1dnud5f</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Do my nails have to be long for an acrylic overlay?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnud5f/do_my_nails_have_to_be_long_for_an_acrylic_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1dnu39p</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>HELPPPP</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnu39p/helpppp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1dntpz4</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press-On Recs? </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dntpz4/presson_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1dntmqr</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shades of Rose </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b88extq9am8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1dntm2y</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and Gold </t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikt5do04am8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1dntlqr</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>suggestions needed: nude</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dntlqr/suggestions_needed_nude/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1dnth7y</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Summer nails, 🪻🏄🏻‍♀️saw inspo pic on here</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnth7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1dnthu2</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Name this shape: inspo vs mine via @pjflux4pulse on Pinterest</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnthu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1dntflf</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Got my nails filled and re-painted today.</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyu019ti8m8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1dnt4jg</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black matte </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q10skjtr5m8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1dnt3wc</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Tequila and lime</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnt3wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1dnt1nv</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Male, grew my nails long, what should I do now?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st5wfpv25m8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1dnsqvo</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brittle nails and nail growth? </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnsqvo/brittle_nails_and_nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1dnsnls</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Opi color - know the name?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnsnls</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1dnqjmk</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you type on a computer keyboard? </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnqjmk/how_do_you_type_on_a_computer_keyboard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1dnsjo0</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Daily oiling 🥰</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnsjo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1dns21m</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Grade my application.</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/abzu5gzjwl8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1dns3n4</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>What’s the best type to do for length and keeping nails healthy?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dns3n4/whats_the_best_type_to_do_for_length_and_keeping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1dnrvtg</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Seeking advice on healing a multi-year split toe nail</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnrvtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1dnrvnd</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>did some pink aura nails yesterday (ft. my soft pink blanket with cats on it)</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnrvnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1dnrpan</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Eh... getting better.</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxfa7myltl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1dnrnmn</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Teal and white marble on a glazed caramel base</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydf9naa8tl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1dnrdfk</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Online nail school?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnrdfk/online_nail_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1dnr8ob</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Green stain/nail advice, please</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnr8ob/green_stainnail_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1dnr627</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>I love my nail tech so much</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjd568m8pl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1dnq686</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for Vacation </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnq686/nails_for_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1dnqyif</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I'm obsessed with how good they turned out</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx9fxc7knl8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1dnqdh7</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Been into JJBA lately, decided to honor a great villain</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnqdh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1dnq65z</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Been playing around with press ons recently 💅🏻</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnq65z</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1dnpysb</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Does UV/LED cured nail glue expire?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnpysb/does_uvled_cured_nail_glue_expire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1dnpupd</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Aquarium nails</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnpupd</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1dnpq6k</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Flower Nails (yes I cheated and used stickers)</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7p9z3bydl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1dnplc9</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello everyone! They told me to upload a photo of my hand so I could ask for a nail model recommendation for a big hand, what do they say? Square or round? </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaaaw67zcl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1dnoxcd</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>New structured gel set. Love the bright neon!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1949gyqz7l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1dnot3c</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Testing out wedding nails! First set - any ideas for any other styles I should try?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbl1a7l47l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1dnoeb8</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Summertime!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppn4llpy3l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1dnoakw</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Help identifying nail colour OPI</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edmakct63l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1dnnm2c</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>How to get turmeric stains out of biab?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnnm2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1dnnu73</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Almond or Coffin?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnnu73</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1dnnqtl</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[OC] Pride nails from PT in Chanhassen! </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k3y8tv1zk8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1dnnqdb</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying Gel Matte Top Coat </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnnqdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1dnnosd</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Shelly Belly</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnnosd</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1dnnlva</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>What shape can I go for with my next appointment to transition to almond nails?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnnlva</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1dnmst9</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this, what do you think? </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lodou042sk8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1dnms37</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Ham!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnms37</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1dnmrbm</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Smallest way to keep nail swatches</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnmrbm/smallest_way_to_keep_nail_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1dnmqyp</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Say bananas 🍌</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flbc9awork8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1dnmixr</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Redid my nails so they’re in regs.</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnmixr</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1dnmhyb</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>i’m just obsessed with this color</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnmhyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1dnmhu1</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>New nails, loving them🫶🏻</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm48x60vpk8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1dnmaek</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Any tips?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4t8kascok8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1dnm4um</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Summer time vibz😎🏝</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnm4um</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1dnm3tz</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>3 years working as nail tech! What do you think?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnm3tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1dnlvrx</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>My nails from December until now.. Which one is your favorite?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnlvrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1dnlutl</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>What do you think of my natural long nails?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnlutl</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1dnlnrt</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>New Set for the Melanie Martinez Concert</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnlnrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1dnldxq</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Yellow's my favorite color 😍</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnldxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1dnlbog</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>My nails grow weirdly</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnlbog</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1dnl9cx</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer ready 🩷  🧡 </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnl9cx</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1dncn81</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I’m new here gang what do i do</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/useyk614ni8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1dnjycm</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Can I put peel off base coat on top of builder gel?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnjycm/can_i_put_peel_off_base_coat_on_top_of_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1dnkmt2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Dip with natural nails for my wedding</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88bcf7g5ck8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1dnkjp4</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>My first DIY gel set. Saved myself a pretty penny</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhpe0i8ibk8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1dnkfjq</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Letting my nails grow: Week 3</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xm6zbtujak8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1dnk682</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Accidental Cottagecore</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnk682</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1dnjsq2</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Press on vs salon dip</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnjsq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1dnykzz</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>“Name Your Polish” from All Mixed Up Lacquers</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnykzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1dny93y</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Listerine green 🧼</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dny93y</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1dnxhc6</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Pink lemonade nails 🩷💛</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs0ftp87bn8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1dnxa8u</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Can I do a layer of peely base under gel polish?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnxa8u/can_i_do_a_layer_of_peely_base_under_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1dnwwsb</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>My turn for the cursed</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnwwsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1dnv45l</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Thinning Starrily polish?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnv45l/thinning_starrily_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1dnunk7</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Grade my application.</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnunk7/grade_my_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1dnuds5</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Magnetics </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnuds5/best_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1dnu76y</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Fresh set who dis</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff0kxwvkfm8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1dntkf0</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>ISO: black polish with pink shine</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dntkf0/iso_black_polish_with_pink_shine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1dnt6c4</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Bringing the grungy juice~</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnt6c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1dnss5a</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn’t decide if I wanted red or green, so I did watermelon </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcmfqnbq2m8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1dnrx4o</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Monday Manicure</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjtm5p0gvl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1dnrdhz</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>My proudest nail art yet: Lemon Nails!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnrdhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1dnq08z</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uncertain </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsrjkib3gl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1dnpwdh</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Please excuse the chip (I am devastated) but I think these are some of my favorite nails I have ever done?!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/belypccafl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1dnps13</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>My first Ethereal polish!! 💛</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnps13</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1dnow10</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Nail Complilation :)</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnow10/nail_complilation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1dnoq98</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Dupe for Twenty pro Collette?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwz86hbk6l8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1dnoivo</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>[Recomendations welcomed] What nail polish is similar to this peach tone?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnoivo/recomendations_welcomed_what_nail_polish_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1dnogcp</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>So excited for to try the new Mooncat x PPG collection!!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n941q4xd4l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1dnns4h</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Having a tough time figuring out how to get my at-home manicure to be as strong as the salon?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnns4h/having_a_tough_time_figuring_out_how_to_get_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1dnnllk</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Shelly Belly</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1wdmi3dyxk8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1dnmzea</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Unicorn Fluff</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnmzea</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1dnmqsc</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Ham!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnmqsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1dnmpqk</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>I'm still new to doing my nails but I'm already obsessed 😊</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gXpXwjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1dnmnbo</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Alien Vibes 👽🛸</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnmnbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1dnlknu</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>OPI- Summer Monday-Friday’s</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07649j13jk8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1dnlj55</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Am I the Only One That Doesn't Cut Off All My Nails When One Breaks?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnlj55/am_i_the_only_one_that_doesnt_cut_off_all_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1dnl2u6</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>ISO dupe for China Glaze Lavenduh! Which is more like periwinkle</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnl2u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1dnkqsv</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Gave my beautiful mom a fresh &amp; simple mani for her upcoming vacation 💕 we love this color on her!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s50c3t3xck8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1dnkkej</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Indie polishes and unmixed pigments</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnkkej/indie_polishes_and_unmixed_pigments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1dnjtlv</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>I used to avoid pale blues but now I’m pretty into them 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnjtlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1dnjlng</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Pure Ice “Rio” dupe?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnjlng/pure_ice_rio_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1dnj1xi</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Pride in pastel 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnj1xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1dnik6m</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Happy Ending and Foot Fetish by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnik6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1dnhzah</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Layered jelly rainbow for Pride month 🌈</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c07evdgjsj8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1dnhdfg</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried stamping, I'm not great at it but I guess it's not terrible </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnhdfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1dnh8pv</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Mourn with me :,)</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnh8pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1dnfle1</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>🌸🐈🌼</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z84188b0bj8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1dnf3sm</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>first nail pic as a new homeowner in my (overgrown) garden 🌼</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cwhwi2b7j8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1dncss2</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Blood red</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l0g82xjoi8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1dnc3ez</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnc3ez/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1dnbgo5</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>swatch request for  OPI Glazed and Amused</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnbgo5/swatch_request_for_opi_glazed_and_amused/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1dnb98m</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>rose water being unreal</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnb98m</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1dnb2ya</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈Future Pride Flags🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnb2ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1dn1hfd</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>essential starter mooncats?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dn1hfd/essential_starter_mooncats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1dnadbo</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Liquid latex recommendations?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnadbo/liquid_latex_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1dn9xmh</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sandy shoreline </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dn9xmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1dn9vgs</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dn9vgs/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1dn9ikb</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>In Top 5 neutrals for brown skin</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dn9ikb</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1dn99re</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Not usually a bright polish person but this feels so right for summer!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sittus0mh8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1dn8grc</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Cirque - Mermaid Grotto</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dn8grc</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1dnzsmk</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>My nails are always EXTRA! 🤣what do you think of the design💕(Done by me)</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/464llp512o8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1dnzftq</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My client loved her nails!! Anything I could improve?? </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnzftq</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1dnz8s2</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Barbie nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr2tlf26vn8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1dnugvd</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>A set I started today~!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmm8hal3im8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1dnsiqx</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Colorshifting eye nail art(done by me)</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8fgie6ce0m8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1dns8x9</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Dark Monarch set I made the other day 🖤</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxgorjm6yl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1dnrwtd</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>did some pink aura nails yesterday</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnrwtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1dnrmmd</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Teal and white marble on a glazed caramel base</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcrreoqzsl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1dnrg9q</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>MellowYellow 🌻</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/419bziljrl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1dnr4u5</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help a newbie! </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dnr4u5/please_help_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1dnqz19</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🫶 finish dayy </t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ythlwjonl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1dnqytk</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>little Bohooos 👻</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnqytk</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1dnq64q</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Cartoon french</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvis1n22hl8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1dnp0w0</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>When you have a cloudy day, it's nice to put a little color on your hands 💟💅</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvui91qq8l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1dnoawl</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gradient effect for the beach, do you like it? </t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3dxtyr83l8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1dnnz7s</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Shellac - looking for color</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dnnz7s/shellac_looking_for_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1dnlrh2</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>loving my nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c17t1fhkk8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1dnkwwr</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maybe my best set yet- blue but smiling </t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnkwwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1dnkjaj</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Koi pond nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnkjaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1dnjpvn</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Long and sharp</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz6saikc5k8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1dnj8ay</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Any haikyuu fans here? (Set done by me)</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnj8ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1dnhmnh</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Instant progress pics</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dnhmnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1dnhece</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Euphoria Nails: a lot of handmade lines😅✨</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lckh439oj8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1dnfszh</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Festival ready 🌸 </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crw1jcqicj8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1dnfh5o</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Wanted to do something demonic 😈</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dssxvy5aj8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1dne4ir</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Beach Nail Set I just did</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53j4lgwozi8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1dndfww</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>butterfly wings 🧡</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hna16vyyti8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1dncnxb</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>brat press ons!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dncnxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1dn9ml8</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>what to do</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yphvwvlqh8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun 26 08:09:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_30.xlsx
+++ b/data/2024_06_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C483"/>
+  <dimension ref="A1:C652"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8644,6 +8644,2879 @@
         </is>
       </c>
     </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1dot7jd</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>French tips are the new it-girls on my fingers!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oysflrkxhv8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1dot5xi</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>I have peeling on the free edge after using rubber gel</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmg92khehv8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1dosthn</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>MOONCAT - Maelstrom</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dosthn</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1doskqi</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>My sister did my nails 😊</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntptqwhp9v8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1dosjp2</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Posting late, but I'm excited about my nails!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dosjp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1dos02v</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Summer nails, oh so cute</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft8ne2qs2v8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1dokjvp</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>New to nails that extend past the fingertip - how do you keep them from flaking or breaking?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dokjvp/new_to_nails_that_extend_past_the_fingertip_how/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1donsc4</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best nail glue for long lasting fake nails </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1donsc4/best_nail_glue_for_long_lasting_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1dop042</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Can anyone ID this polish or a dupe? It’s so incredibly pretty but also probably at least 15 years old and I have absolutely no idea what it is because the bottle has no name label!!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dop042</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1doqdmx</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Hi!☺️ This is my first post ever!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxju6k47ku8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1dor8oa</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Summer days called for a fun summer color</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc35aljqtu8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1doqyo7</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This nude didn’t go well with my skin tone, cute set overall!! She mixed a few nudes together </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yb18kblqu8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1doqxu5</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The spider was my absolute favorite part of the set hahah I love Halloween nails </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag0f0vtbqu8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1doqkk0</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>My latest set I’ve done for myself</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8bici07mu8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1doqcwo</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are you using for press on nails? </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1doqcwo/what_are_you_using_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1doqbvw</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ocean themed set for summer I just made </t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nihu50oju8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1doq700</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Nail drill recommendations...</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1doq700/nail_drill_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1dopzgy</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>first ever acrylic set on myself!!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rujraunvfu8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1dopky3</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Did mine and my bsfs nails (I have to clean mine up some more)</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dopky3</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1dop2bk</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>I liked the butterflies but they eventually fell off which was annoying lol</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pu0dbcp6u8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1dop03y</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Chappell Roan inspired nail art 💜</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aoey86f46u8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1dopeh3</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer chic nails </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qaukh41au8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1dopcak</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Loving this color always!!✨</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucqxtfef9u8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1dop59t</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>How to fix my broken nail?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ja4829j7u8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1dooz11</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set from my nail artist </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dooz11</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1dooguf</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Passion Pink</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aviz6ujv0u8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1doogf4</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>I’m just gonna keep practicing!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doogf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1doo4lm</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Got a new set yesterday😌 I love aura nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhgg2zxuxt8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1donkue</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>French Ombré</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2lr1wrzst8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1donjt8</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Is there a way of requesting thickness when getting a Shellac manicure?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1donjt8/is_there_a_way_of_requesting_thickness_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1donhms</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Can you give me nail suggestions?? I want to have prettier hands!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x7fuei7st8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1domk6c</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Obsessed with my Nanami Kento themed nails 🥹</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zwvylvtjt8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1domc3b</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Hello, i got my first set of nails today by my mom! what do you think 🥹</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7io79njrht8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1dom4vi</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>First time self gel</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed16r2awft8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1doludy</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>In love with these!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doludy</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1dolpjz</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Cute?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k9sbxj3ct8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1dolo12</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Is builder gel and UV gel the same thing?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dolo12/is_builder_gel_and_uv_gel_the_same_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1dodjeb</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Maybe pushing back cuticles doesn't actually change how they grow back (details in comment)?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja0ljf4vjr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1dojxzl</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Can’t get peel off base coat + glue on nails to work 😭 help??</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dojxzl/cant_get_peel_off_base_coat_glue_on_nails_to_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1dolcyr</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Never gotten a French gel manicure before and I love it. 🐬</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qkejff19t8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1dol2l8</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Gel X, how’d I do?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n5wa5yh6t8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1dol09i</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>What shape are these?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dol09i/what_shape_are_these/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1dokt0e</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>What does this mean when it happens?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/68s56lb44t8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1dokpbl</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>New nail set!! 🍒</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dokpbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1doklxe</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Bathroom lighting but still bomb nails 🧡🍑🍊</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doklxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1dokc0y</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Charms and tattoo stickers</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dokc0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1dokbtr</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Pink Lemonade 🍋</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dokbtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1dokbg3</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Loving summer nail colors</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhb9p5t40t8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1dojk2j</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How long do press ons last? </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dojk2j/how_long_do_press_ons_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1dojckc</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Chrome shimmer help</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cppm0efbss8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1doj5c9</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails are completely destroyed after abusing them with acrylics. </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1doj5c9/my_nails_are_completely_destroyed_after_abusing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1doixvf</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>LINCOLN PARK AFTER DARK ALL YEAR ROUND 🖤</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doixvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1doirdl</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>nail charm keeps snagging</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doirdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1doikop</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍒 summer vibess </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sr5noys7ms8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1dohj42</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>BIAB lifting</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dohj42/biab_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1dohgod</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Press on glue that doesn’t ruin them?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dohgod/press_on_glue_that_doesnt_ruin_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1dohfbc</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>lucky lucky lavender</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tt8zejgds8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1dohdh7</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>LDS gel reviews??</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dohdh7/lds_gel_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1dofmzy</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>European Peel Off Base</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dofmzy/european_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1dogrdw</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Too flat?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dogrdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1dogb71</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before and After </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iztkxjr45s8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1dog2w8</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Mooncat in Devil’s Ivy</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3wjkvzjf3s8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1dofz8k</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pretty summer nails </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3myzdf4o2s8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1dofnaf</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>beginner nail artist (started in april) and I think this is my favorite set yet!</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dofnaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1dof4dv</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>are these cute? my sister and one of the besties don't like them and i'm insecure abt it 😭</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3vvohpdwr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1doeutz</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling the summer vibes </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doeutz</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1doepwb</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Matte pink(ish) press-ons 🩷</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njdxb16asr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1doe7gu</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Cracking up. Have been thinking for days about what vibrant colors I was going to get on my nails. Walked out of the salon with Funny Bunny &amp; Bubble Bath 😂</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7svrk8udpr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1dodzpu</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Summer set✨🫶🏼</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dodzpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1dodx9i</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Simple yellow acrylics at my local salon. What do you think?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dodx9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1dodjp7</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hi new here. how am I doing? </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0tyfbblkr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1dodckc</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Pride nails! 🌈❤️</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dodckc</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1docoo9</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I've been loving my press ons lately</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1docoo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1dociw4</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>I've always had square nails and one day I decided to file my nails almond and now I can't decide what looks better on me. Does square or almond look better? I want my fingers to look slim and less chunky.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dociw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1dochx2</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They turned out beautiful </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkbo2uovcr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1docgcm</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Anyone have any Taylor Swift nail designs!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1docgcm/anyone_have_any_taylor_swift_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1docc0a</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Neonails shade for Essie ballet slippers</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1docc0a/neonails_shade_for_essie_ballet_slippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1doc828</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you don’t want to spend $120+ on a mani and pedi for your beach trip so you do it yourself at home. Not as good as the nail salon but it’ll do. </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ossi1m1var8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1dntooo</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Advice on how to get your nailbed skin to grow OUT?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dntooo/advice_on_how_to_get_your_nailbed_skin_to_grow_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1dnu55u</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Needing witch-y inspo! Show me your edgy nails. </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dnu55u/needing_witchy_inspo_show_me_your_edgy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1dnvz1c</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63bs2cl7wm8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1do7dlt</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Allergy - press ons?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1do7dlt/allergy_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1do9hdk</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>What is a good treatment to give your nails after taking off builder gel/gel polish?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1do9hdk/what_is_a_good_treatment_to_give_your_nails_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1dobnxu</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying something fancy! </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dobnxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1dobn7t</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Finally sat down to do my own nails - not perfect but I had some time to do an extension and something not black 🤣</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1mdkb5f6r8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1dobjq4</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Neon red mani w/ a subtle glitter 🔥❤💅🏽 done myself, on my natural nails! I'm proud of these</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dobjq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1dob711</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Today I did a total black</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yqf9z303r8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1dob0uf</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help findimg a nail salon </t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dob0uf/help_findimg_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1doay9i</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Selfmade nails- is the nude fitting me?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doay9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1do0vzt</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Should I give my nails a break</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4b8xkqm1go8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1do1paa</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Nails in Paris ✨</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do1paa</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1do37zm</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>why does my mirror gel do this? how do i fix it?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do37zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1doas29</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>new blue hibiscus nails!!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dutfn6pxzq8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1do5pm8</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Press ons, Gel polish starter recommendations ( help I've spend hours browsing subs at this point)</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1do5pm8/press_ons_gel_polish_starter_recommendations_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1do9dll</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Does anyone know where to find OPI Chrome Effects in Tin Can Man</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1do9dll/does_anyone_know_where_to_find_opi_chrome_effects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1doapze</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Obsessed with my new iridescent nails that gives off different colours depending on the lighting!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doapze</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1doao1x</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Custom plates for nail stamping?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1doao1x/custom_plates_for_nail_stamping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1doanvj</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Yuck with my nails</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doanvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1doa2s4</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Pride nails I’ve done so far this month!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doa2s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1do9wxk</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer vacation means getting new nails. </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do9wxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1dosoaw</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>MOONCAT - Maelstrom</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dosoaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1dosib7</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>I slept on this</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dosib7</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1doraoh</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Self-Care Sundays: DIY Manicure Edition</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1doraoh/selfcare_sundays_diy_manicure_edition/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1doqr9t</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>🦇🦕🐈‍⬛ Et tu, Brucie? 🐈‍⬛🦕🦇</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doqr9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1doqcyn</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Mooncat Cheshire Cat 💜😸💜</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doqcyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1dopkl7</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Having a big moment with Sassy Sauce Blowin Bubbles recently! 🫧</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dopkl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1dopjrf</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>I Call This Red Porcelain</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dopjrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1doowak</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Could anyone possibly identify this polish? It is very old and has no front label! It’s the most gorgeous glazed pearly nude (photos of the bottle included)</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doowak</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1doosuv</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>glitter nails ✨</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doosuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1doosdx</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Dimension</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/of66jk624u8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1do42lt</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Grade my application</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cvsnfygmhp8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1donf51</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Is it just me ?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1donf51/is_it_just_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1doi29g</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Loving thermal polish!</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1doi29g/loving_thermal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1don9bl</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Lemons in to Lemonade</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q56b5y3qt8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1dol8jh</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Flower Child makes every mani 10x better</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dol8jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1dol3dv</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Summer 2024: Quiet Dreams</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dol3dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1dokyih</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>painted my nails again after a 3 month break</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dokyih</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1dokc8k</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>May have done some damage. Oops 🤭 (should I do some swatches??)</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dokc8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1dokawh</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Pink Lemonade 🍋</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dokawh</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1dok9cj</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Rapid Red ❤️</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dok9cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1dojxff</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Has anyone successfully fixed overgrown hyponychium?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dojxff</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1doj9lp</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Lion with a Thorn in it’s Paw</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzwpyjrnrs8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1doiwqd</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need Nail Ideas- Wearing this dress to a vintage prom </t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o82t2vauos8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1doivk3</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>A sweet little matte/glossy French Tip :)</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doivk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1doidjm</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Quiet Dreams - DVN</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doidjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1doia1h</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>“Bottled Rage” from Mooncat</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doia1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1doi7bu</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>I wanted to do something light and reminiscent of summer! (excuse the cat hair and the paint steaks lol)</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doi7bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1dohn9r</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why yes, I WAS eating cheetos and crafting with glitter. How did you know? </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dohn9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1dohadv</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell sparkle bomb</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dohadv</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1dogmiz</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Plankton + Read Between My Tulips</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctzmep1j7s8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1doghaj</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Comparisons</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doghaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1dofxa6</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Sun Catcher/Hardware vs Forces - EdM</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dofxa6/sun_catcherhardware_vs_forces_edm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1dofncp</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Thermal nail polish question: Fancy Gloss Barbie 2.0 alike</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dofncp/thermal_nail_polish_question_fancy_gloss_barbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1dofmfm</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>My first green nail polish in my life and the longest nails I ever had</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8opyzo20s8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1doduyc</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Rainbow Road 🌈  🌠</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s1o0ahtmr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1dod7uc</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Looking for a drugstore bubblegum pink creme</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huc36q65ir8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1dobd2x</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Mooncat- Not Today Satan</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dobd2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1doajbr</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Bi Flag: Pride Flags for Pride</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doajbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1doa3si</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Dupe for ILNP Juliette?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5g51kdsuq8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1do9zsa</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Put some holo on it</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do9zsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1do8z0x</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>ILNP ultra chrome skittle + holo french tips :D</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3w3rwbe9mq8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1do8iqr</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Pride water marble. I've created awesomeness!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9zz2xrzriq8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1do831b</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Painted Polish and Cupcake Polish?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1do831b/painted_polish_and_cupcake_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1do7w9v</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Pride mani</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uxlr616eq8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1do7vjx</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>The sponge gradient looked good until I tried to remove the latex layer protection around the nail :c Tips? A good brand of latex to try? Another protection layer method?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ygdhtr0eq8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1do7gvz</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>7 layers may have been excessive 🤣</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do7gvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1do6wyh</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>One side of my nail naturally grows “flipped.” Is there anything I can do?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do6wyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1do5ma6</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>How can I fix my nail bed?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do5ma6</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1do4b4i</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Pushed proximal fold too far back?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0yihem1kp8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1dnv3cw</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>What I ordered, what I received, and what I got as a replacement</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dnv3cw/what_i_ordered_what_i_received_and_what_i_got_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1dot9uo</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Wonyoung from Ive if she were  nail set(done by me)</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9oaa7d2qiv8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1dosq5h</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dosq5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1dosoua</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Which green would look better with unicorn chrome?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dosoua</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1dor4nn</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>beach / ocean themed gel press ons i just made for summer 🌊🐚🦪</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czklpkshsu8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1dojx9s</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Always shines ✨</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dojx9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1dojf0u</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Nude nail polish and glitters</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxwjaveuss8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1dohvgd</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Seeking Advice on Best Korean/Japanese Gel Sets for Aspiring Nail Tech</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dohvgd/seeking_advice_on_best_koreanjapanese_gel_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1dof9e9</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Do you like this style of nail decoration?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kil8s53fxr8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1doc6fs</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Newbie! First set of 3Ds on myself!</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doc6fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1do9siv</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Am in Love </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8708r4gsq8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1do9s0j</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>and what do you think? perfect</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k5kd7hcsq8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1do9r4d</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Inspired by wedding dresses</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkoxzvn1sq8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1do9lrj</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Spongebob's irregularly shaped</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bfszej0rq8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1do798w</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tell me they're not perfect.. &lt;3 </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tns38mkb9q8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1do6rl6</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>little clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrvphsxf5q8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1do608v</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Help. The sticker is bubbling.</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p0rp0xazp8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1do5gbw</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>I love simple nails 🤍</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5joovfjup8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1do5ecc</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do5ecc</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1do2ms9</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this work of art </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1do2ms9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun 27 08:09:16 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_30.xlsx
+++ b/data/2024_06_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C652"/>
+  <dimension ref="A1:C807"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11517,6 +11517,2641 @@
         </is>
       </c>
     </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1dpkyg6</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>SET I DID THIS WEEK !!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpkyg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1dpkws2</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Did I do that???</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2veyfq61a29d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1dpkpq7</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Press on advise</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpkpq7/press_on_advise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1dpjj55</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time Acrylic Nails </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpjj55/first_time_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1dpj4ap</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Nails for next few weeks</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/733d33fgp19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1dpiwr0</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93micv39n19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1dpic9g</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Tried Gel X for the first time</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txhececch19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1dpi0bu</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Love these so much! Meow!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2c560c5e19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1dpe6p8</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Gel or lamp allergy? SO CONFUSED.</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpe6p8/gel_or_lamp_allergy_so_confused/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1dp86y3</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>“natural” feel press on recs</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dp86y3/natural_feel_press_on_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1dpfqrw</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>gel polish lifts after a few days on natural nails</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpfqrw/gel_polish_lifts_after_a_few_days_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1dphs60</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Care Bears nails I did!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5oje0t4wb19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1dpe4ia</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Nail Help</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpe4ia/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1dphckj</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Why does my chrome powder wipe off after applying top coat?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wuztr4p719d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1dphnep</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Opinions? I’m pretty proud of this set, tbh.</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ln68h9pla19d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1dphjot</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Wedding nails dilemma!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dphjot/wedding_nails_dilemma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1dpgos9</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>So wish I could have longer nails at my job 💔😔</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz91fgpd119d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1dpgrdw</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Middle fingers?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpgrdw/middle_fingers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1dpgkps</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I can't have acrylics and want nails that last 2-3 days</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpgkps/i_cant_have_acrylics_and_want_nails_that_last_23/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1dpgd60</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they look uncomfortable but I love </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtm6cnggy09d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1dpf662</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Which nail shape looks best on my hand? Square/squoval or round?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpf662</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1dpeygw</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I just finished these My Melody nails☺️</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5nzp6ptl09d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1dpengx</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Birthday nails 🌊🩵</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbqrz5m2j09d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1dpdjp4</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Photoshoot for my birthday nails because my tech went off</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpdjp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1dpc371</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>After two weeks my nails look like this…</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i939j3zaxz8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1dp2twx</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Toe nail fell after gel pedi</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dp2twx/toe_nail_fell_after_gel_pedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1dpdvqy</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Black nails today ~</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ba0ynz5ac09d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1dpdqiq</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>First try at portrait nail art (Sabrina carpenter)</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3kb52mdza09d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1dpdpk8</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>3D Press on Nails</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpdpk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1dpdg9s</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Removing nails before surgery and putting them back on </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jinw12qm809d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1dpdd7m</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Groovy</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpdd7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1dpd71q</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Are these nails too tacky for my engagement photo shoot? I have 2 days to get them redone if needed</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpd71q</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1dpd5ml</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>My first set of nail art ever!!!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i81nkw32609d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1dpcp91</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Grateful Dead Nail Inspiration (pics are from Google and a Facebook group; not mine!)</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpcp91</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1dpcrod</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>mermaiddd!!!!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1wddzzq209d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1dpchx4</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Had very high hopes for this set that I made, i super disappointed rn</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75z1mpti009d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1dpa498</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>pride nails!! hard gel fill 🦄</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpa498</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1dpacrf</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Sally Hansen has a $6 holo line but… top coat ruins it</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpacrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1dpc6n3</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>i love my nail tech!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpc6n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1dpajew</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>One piece inspired nails!!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpajew</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1dpbfvo</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Octopus inspired nails</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpbfvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1dpc0b4</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>24k gold leaf</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwckowwlwz8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1dpbxzt</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>I painted my nails red!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpbxzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1dpbwdc</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Experiences</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkvsjr8rvz8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1dpamtk</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Do I really need flip flops for a pedicure?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpamtk/do_i_really_need_flip_flops_for_a_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1dpa919</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>US Army National Guard nails to honor my grandfather</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpa919</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1dp8id1</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Show me your proposal/engagements nails x</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dp8id1/show_me_your_proposalengagements_nails_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1dp7x55</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“goth nails plz” </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy8xp4ek1z8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1dp7cxs</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Excited to play with cat eye polish again!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yvmwsx8hxy8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1dp6z3u</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Did them myself without any acrylic or gel!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h1ecennuy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1dp6rr4</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Got my nail done and I love them 😍</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dm5k7i6ty8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1dp6kaw</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Probably the cutest set I’ve ever had 🍓💕</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp6kaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1dp6f94</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Bright pink set on my natural nails 🩷</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n64ij3vqqy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1dp4d4n</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Should i get french next on this shape?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp4d4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1dp0f6y</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>My nails after my appointment yesterday 😭</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln8cqz9jix8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1dp5ykt</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>My niece wanted to have nails like mine😂</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doxobcl7ny8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1doz3t6</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>First time DIY gel enhancement</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doz3t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1doyh1t</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>builder gel peeps! what happened when you fully removed your builder gel?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1doyh1t/builder_gel_peeps_what_happened_when_you_fully/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1dowicv</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>I need your opinions &amp; advices</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dowicv/i_need_your_opinions_advices/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1dp5tog</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish thinner is AMAZING </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dp5tog/nail_polish_thinner_is_amazing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1dp5rxj</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Do these look as bad as I think they do?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp5rxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1dp5l3w</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Orange peel texture a few days after gel manicure?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l3yx6ieky8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1dp5jx2</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>St. Patrick Nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p87wqld6ky8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1dp5eit</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Easter Nails</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqvapj31jy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1dp5cyn</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French Glitter Gradient </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnrupqjpiy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1dp56m7</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frac6a2ehy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1dp4wh2</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Cuticle nippers</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dp4wh2/cuticle_nippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1dp4ubb</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Got my Pride mani in under the wire</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spmjykwvey8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1dp4jdv</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails, thoughts? </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/963h88llcy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1dp4her</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Chrome tips look curdled?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7j54v4h7cy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1dp4bno</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Love my Kiss Salon XTend Nails!</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9igq5e41by8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1dp4bhc</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>You know it's a good set when they're used to advertise. I'm in love!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp4bhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1dp495r</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Birthday nails !!!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oit95mwhay8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1dp2ncs</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Inspired by someone else's post on here!! Bonus pics of my friends nails ♡</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp2ncs</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1dp3s9r</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Chrome rainbow for the last few days of Pride month 🌈</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdf2dqo07y8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1dp3ryt</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a specific type of orange polish </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dp3ryt/looking_for_a_specific_type_of_orange_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1dp3eu2</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>My birthday nails!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp3eu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1dp30fg</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Fresh summer set 🌞</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39znseob1y8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1dp2sl5</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>My first set I’ve had with Gel X</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvuq3drpzx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1dp2qni</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>builder gel 🥰</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghaw7rxbzx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1dp1zf3</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>My favorite gradient I’ve done so far 🌈❤️</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri0y2ga1ux8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1dp1q2p</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>New Pink Cat Eye Nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0g5nn4o1sx8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1dp1qcw</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>I liked them at first but now I’m not sure 💕</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp1qcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1dp1oqp</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Feeling ready for the 4th</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp1oqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1dp1n0b</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Wanted something more summery for the warm weather, feedback welcome :)</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3grpmcirx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1dp1kiu</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Cherry nails 🍒</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp1kiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1dp18r2</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>indeed, I’m obsessed 🌹</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp18r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1dp0xab</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>My wife’s nails</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08cbz6ucmx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1dp0h8o</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Natural nail question - Is there a certain shape or anything I can do to make them look a little cleaner/more sophisticated?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp0h8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1dp06t8</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>what products to use to recreate this (same colours)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phemjrrrgx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1dozsfs</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Cutting off my growth today</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ij2cilmdx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1dozeax</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Getting surgery soon!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dozeax/getting_surgery_soon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1doyx6a</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Jelly nails with French tip</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s4l90up6x8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1doythc</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>In love with my new sets 🥹</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxe98n5v5x8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1doypcl</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Trying out TWO accent nails 😱😂</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex00wn8w4x8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1doyd4a</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Loving this color always!!✨</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doyd4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1dox5p4</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Painted a few new unlikely friends on my nails</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehzut3ferw8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1dowknp</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Trying to find a brand of nail polish!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dowknp/trying_to_find_a_brand_of_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1dovmwc</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>What are your opinions?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6tx86rybw8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1douhhd</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Freehand flowers</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snkr2js6yv8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1dphzoq</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Nail Care Advice</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dphzoq/nail_care_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1dphsn7</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Dupe for Painted Polish's "I love you berry much"?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dphsn7/dupe_for_painted_polishs_i_love_you_berry_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1dphryu</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t xml:space="preserve">brat green recommendations? </t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifrkf7bub19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1dphozm</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can anyone recommend a really good top coat? </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0sldqvza19d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1dpgyh8</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>This polish satisfies my inner evil queen</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpgyh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1dpftne</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>My BKL Elden Ring selections!!</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6wtxlunt09d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1dpf0xk</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Summer nails are here 💙💙</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpf0xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1dpewa9</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Took me way too long to try this one! 🧨✨</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpewa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1dpea3u</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gemini (The Twins) </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6b18ko0of09d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1dpe64w</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>I layered ILNP’s flower child on top of Cirque Colors Sol, and I’m OBSESSED with the results!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j37bmu8pe09d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1dpdd6x</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Why do the edges of my builder gel disappear? I’m using Akzentz Trinity hard gel, I apply it right up to the cuticle but it seems to evaporate away. Am I just moving too slow?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om2loiyv709d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1dp16fk</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can someone help me </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcpauy07ox8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1dp9vsy</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Chaos Skittle</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp9vsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1dpaga3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fine, it's worth the hype </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hz4qy2jkz8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1dpafnu</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Where to buy collectors/vintage polish?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dpafnu/where_to_buy_collectorsvintage_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1dp9ik5</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>June manis!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp9ik5</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1dp9f4g</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">one specific nail bed always recedes </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dp9f4g/one_specific_nail_bed_always_recedes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1dp8znr</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Starting over 💔</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp8znr</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1dp8qsx</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neutral Gel (LED) Color Recs? </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubdpu8ys7z8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1dp7jf2</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I think you already know what this one is 💜</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsk02mpsyy8d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1dp6l3m</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Hey Mercury, Can You Not?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u0duz34ury8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1dp5gpn</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Cirque XOXO Jelly vs ILNP Malibu color comparison?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dp5gpn/cirque_xoxo_jelly_vs_ilnp_malibu_color_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1dp4o24</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>New to doing my nails and tried oval shape for the first time last week, do they look 'off' or am I overthinking?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp4o24</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1dp4jci</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t xml:space="preserve">airbrush babies by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i86mj6flcy8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1dp422u</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Cirque colors High Society 💚</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2fi0br19y8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1dp309e</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Help finding a dupe! Cirque - Narcisse</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp309e</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1dp2ne8</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ancient Julep Skittle </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp2ne8</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1dp2k22</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Eyeshadow used</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dud0y1zxx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1dp1bjr</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>To everyone with long nail beds who breaks a nail, this is a reminder it could be way worse 😭</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fhiciu6px8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1dp0hyz</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>My Pride nails</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvxsf005jx8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1dp0hra</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Lotions with jojoba oil infused</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dp0hra/lotions_with_jojoba_oil_infused/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1dp03ln</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Just keep swimming ~ fishy manicure</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp03ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1doyrao</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>How did this make it into a "pruglies" collection??</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8uxsdsc5x8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1doynt6</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Starting as a new artist</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1doynt6/starting_as_a_new_artist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1doyl0b</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Loud, Weird, Gross Cicada Summer Mystery Polish from Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doyl0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1doy4h0</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Not my best combo...but</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1doy4h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1doww40</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>With Sprinkles 🍩</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6ph9zsvow8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1dowqda</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>For Buttercup apples</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dowqda</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1dou375</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Gel like top coat recommendation?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dou375/gel_like_top_coat_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1dotg8f</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>BKL - Let's Give Them Hell</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dotg8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1dpllys</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It looks beautiful and always shines </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfn0h8lqi29d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1dpfv9h</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1zy2wxmrt09d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1dpfbc6</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Very coquette💜</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpt43la3p09d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1dpdpua</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try at portrait nail art (Sabrina carpenter) </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nqyepigta09d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1dpc9qg</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>any tips on sketching with nail art</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpc9qg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1dpa3lv</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Hand painted fruits and veggies and sculpted sushi 😅</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpa3lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1dp5to1</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Might be too long for some people but it’s majestic (done by me)</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp5to1</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1dp5tgw</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did these last night! The petals &amp; “stone” are solid gel, gel polish, &amp; hand painted! </t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avouwcv4my8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1dp5noh</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>trying to make press on nail sets for myself. anything im missing in the list, anything i should drop?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dp5noh/trying_to_make_press_on_nail_sets_for_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1dp3goz</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I wanted to show off my hand painted flowers too!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp3goz</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1dp0ych</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Summer camp nails!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1jpca23jmx8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1dp0d9f</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>summer nails 🧡🌼</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp0d9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1dp0cmi</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>I can't believe how beautiful these nails are. I was fascinated 😍</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dp0cmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1dox0ap</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Nails of the day</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guc9giozpw8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1douh7c</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Freehand flowers</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdctvnv2yv8d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun 28 08:08:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_30.xlsx
+++ b/data/2024_06_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C807"/>
+  <dimension ref="A1:C981"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14152,6 +14152,2964 @@
         </is>
       </c>
     </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1dqdeyx</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>How long is too long to go in for a fill</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqdeyx/how_long_is_too_long_to_go_in_for_a_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1dqdda8</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>First gel set ever? How did i do?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqdda8</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1dqarx8</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Nail splitting! Helllpppp!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqarx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1dqcx2c</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I literally cried after this set🌺</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqcx2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1dqaa2s</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Would you trust a nail tech working out of their home?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqaa2s/would_you_trust_a_nail_tech_working_out_of_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1dqcjaj</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>wich design u like the best</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqcjaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1dqchws</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Current set </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqchws</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1dqcgyo</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfshfcue499d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1dqbru7</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Structured gel &amp; oily nails</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqbru7/structured_gel_oily_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1dqbkkn</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>We match</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgtr03hgu89d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1dqatgt</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Who love charms?? Would love inspos. </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqatgt/who_love_charms_would_love_inspos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1dqa8ez</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>It’s giving minimalist Independence</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueqc6t20h89d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1dqa55r</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Is this a good base nude for my skin tone? I bought it singularly, based off of review photos, but I’m new to doing my nails and can’t decide if it’s a good match for me</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6f0q845g89d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1dq9s08</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me? Square or almond</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq9s08</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1dq9kqu</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Trying to achieve an elegant, clean girl nails look. I think my nail tech did pretty well on this one.</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4v5ttxsa89d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1dq9fay</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>What color nail polish is this?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq9fay</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1dq9bbl</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>How would you time your nails for this?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq9bbl/how_would_you_time_your_nails_for_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1dq99hi</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did them myself with softgel and use solid gel, they last 1 week and I already lost one. How can I make them last longer? </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq99hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1dq98p7</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>another ocean set ✨🩵</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q005xgcq789d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1dq8yh0</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Again</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq8yh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1dq8ygl</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Money press-ons</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq8ygl</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1dq8szl</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My pic vs insta nail inspo pic from @nailsbybrook___</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq8szl</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1dq8mge</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Feeling savage</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyp0tj3u189d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1dq8h45</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>4th of July Nails! (Set by me)</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq8h45</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1dq8fx6</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j7bosq6089d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1dq86ja</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Should I redo them?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq86ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1dq88j4</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Help me pleeeeease</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq88j4/help_me_pleeeeease/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1dq88be</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful nail art </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwatrp49y79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1dq7ypr</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new "neutral". I swear it matches everything 😜 (much thanks to my helper) I painted the underside to match </t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq7ypr</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1dq1lgl</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Builder gel - what to do when it grows out?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq1lgl/builder_gel_what_to_do_when_it_grows_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1dpp4xn</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Creativity issues</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpp4xn/creativity_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1dq7i7g</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Color dupe?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq7i7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1dq7gg8</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Yes or no ?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0k6zqviq79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1dq73qq</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3iarnj0gn79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1dq6nw2</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I just needed some nail lovers to bare witness to the cutiest nails I've ever gotten! 🥹☁️🫧</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq6nw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1dq6l0d</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>prom nails💙</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq6l0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1dq6id5</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>juicy pink sea glass 🌊🐙</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq6id5</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1dq6f16</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Would you date a guy with nails like mine?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v70fsrdch79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1dq6eod</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>nail influencers on youtube</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq6eod/nail_influencers_on_youtube/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1dq653b</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Subtle but still festive.</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq653b</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1dq5tc3</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gems and jewels 💎 </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq5tc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1dq5rgv</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Rainbow nails 🌈</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq5rgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1dq5eio</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Nail probs</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq5eio</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1dq59a1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>swirly pearly 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gr3yy86k779d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1dq54l1</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Nothing fancy, just wanted to add some sparkle to the weekend</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o23u3kf679d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1dq50vt</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Destination wedding nails were my fav so far!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl6o4wtk579d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1dq48p1</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Love a fresh set x</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojlf9eb3z69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1dq47r1</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>press on nails I last week!!!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq47r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1dq3wx4</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Gel x for an upcoming wedding☺️</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq3wx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1dq35rg</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>shell nails I did for myself!</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq35rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1dq333g</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Am I the only person that hatessss press ons</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq333g/am_i_the_only_person_that_hatessss_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1dq2zx1</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Best service for natural nails?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq2zx1/best_service_for_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1dq2m4b</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Nail help</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8k0ih0e9m69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1dq2en1</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Flames bag/ flames nails 🔥🤘🏻</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yt6krqnpk69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1dq28u4</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>my 3rd set on a client 🥹</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq28u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1dq23v0</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X fill </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dq23v0/gel_x_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1dq1qny</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>First time ombre! Done by me</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ik8g21kf69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1dq1kp5</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Are these almond?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejtopnvce69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1dq0zp0</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>JUST STABBED SOMEONE HALLOWEEN NAILS 🎃</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tuou0h5a69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1dq0xrq</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Nails a month ago</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn4egp2r969d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1dq0sm3</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>what shape of nails should i do</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq0sm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1dq0b6r</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Just trying to better my nail game</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fxh7h52569d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1dq08e0</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Ready for 4th of July ⭐️🇺🇸</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq08e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1dpz3hf</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>On a nail health journey!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpz3hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1dpxe15</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Orange-you glad it’s almost the weekend 🤭</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpxe15</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1dpy1cd</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions on the French </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpy1cd</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1dpyi7c</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My all-time favourite. </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8k6xlkejr59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1dpz8oe</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>New nail set✨ what do you think? :)</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpz8oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1dpyz3b</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Pride Month Nails</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igjg5u90v59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1dpyxym</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails, I’m not sure about this one </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8lf90iru59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1dpym59</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Crawling ants set by @Liz_Nailing_It in Wilkes-Barre, PA, USA</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpym59</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1dpyhrr</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Dewy succulent nails for my bestie’s bridal shower this weekend (“Let Love Grow” theme) 🤭🪲💧💚</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpyhrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1dpyeh5</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Semicured Gel polish</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpyeh5/semicured_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1dpyawo</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>I call this mani traffic cone chic✨</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/050ef5i1q59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1dpya0t</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>do male nail techs comment on the looks of female clients?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpya0t/do_male_nail_techs_comment_on_the_looks_of_female/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1dpy61o</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Never too old for mermaid nails(set done by me)</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpy61o</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1dpy1ue</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I love this set!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpy1ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1dpxunw</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Is this a bad nail job or am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpxunw</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1dpxdbn</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little summer fun! </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ecxzdo4j59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1dpsd9i</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>New in the game+ need help</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuewv4yth49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1dpx0qh</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in ages and I’m in love 💕</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpx0qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1dpww0c</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>MMA with dip?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpww0c/mma_with_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1dpwo5f</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Prom nails</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpwo5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1dpwfc8</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Recent sets I did ݁₊ ⊹ . ݁˖ . ݁ ᯓᡣ𐭩</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpwfc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1dpw8an</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Palm trees pedi</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpw8an</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1dpw7g1</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Get a fill or wait?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4i5htrma59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1dpw7b6</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>What would a top coat of translucent jelly gel look like with a bottom coat of sparkle or chrome?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpw7b6/what_would_a_top_coat_of_translucent_jelly_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1dpw5qq</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>How can I improve my nails?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2s2ukt9a59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1dpw5ee</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Professional/work appropriate nail suggestions? </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpw5ee/professionalwork_appropriate_nail_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1dpqan7</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Some blingy frenchies</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8g459md049d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1dpr2b0</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Advice from other nail techs?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpr2b0/advice_from_other_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1dpvpkm</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Blue is the chosen color of the week 😎🌀😎</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpvpkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1dpuvz0</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Current nails, they get changed on Sunday to 4th of July designs</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imqipwdw059d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1dpurzo</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 6 year old decorated my nails. Upncoming nailartist! </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuwqj0b4059d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1dpuddj</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Guide for understanding nail services and treaments?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dpuddj/guide_for_understanding_nail_services_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1dpu9kx</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I like the red just a 🤏 more</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpu9kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1dpu5t2</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She wanted neon everything! </t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3u4zkjlbv49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1dptwqn</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Advice?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dptwqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1dptvuw</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Pedi or Mani First?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dptvuw/pedi_or_mani_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1dptqll</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Top coat recommendations</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dptqll/top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1dqdhsx</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Rest in pieces</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqdhsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1dqdgxt</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Broke my nail, is it possible to be repaired</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2b4uy8bg99d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1dqcnya</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Having my nails done seriously changes the way I feel about life</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqcnya/having_my_nails_done_seriously_changes_the_way_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1dqbus9</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail splits up the center, need help! </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqbus9/nail_splits_up_the_center_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1dqa91o</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Havent done nail art in a while!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqa91o</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1dq93tz</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>ILNP/USPS sent my order to the wrong address? :(</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dq93tz/ilnpusps_sent_my_order_to_the_wrong_address/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1dq7ra8</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>A Small Canmake Haul</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw6q8n9nt79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1dq7h3b</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>🐍</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfqawz4vq79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1dq6b2l</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Unpopular opinion? Seche vite is my fave topcoat</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1t9iepdg79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1dq5nje</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Straw-Buh-Buh-Buh-Buh-Berry</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hai36mnva79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1dq5mm7</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Went all-in on my very first nail polish purchase</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01jl1c4oa79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1dq4xs4</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Help with Impress Press on Nails (the no glue kind)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dq4xs4/help_with_impress_press_on_nails_the_no_glue_kind/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1dq4ukt</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Cursed Cat</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq4ukt</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1dq49wi</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>A big lump with knobs</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpqjyekdz69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1dq441q</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>The horseshoe magnet scares me but I tried it anyway</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j03pnt3wx69d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1dq420r</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lts7se8jx69d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1dq3qzh</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Ideas for Essie Jag-u-are</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dq3qzh/ideas_for_essie_jaguare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1dq3p2v</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Paradox Polish</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq3p2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1dq32fe</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>My little brother asked me to paint the nails on his left hand!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfssea9pp69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1dq3271</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Cirque unlucky bag</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un2js1dnp69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1dq2jby</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Sabertooth with Moondust ✨</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq2jby</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1dq2jbs</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>What non-gel formulas last as well as Essie Jelly Gloss? I applied this 12 days ago!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdiz1tg1l69d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1dq2bys</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>A little sparkle fixes everything ✨</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq2bys</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1dq29em</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>This GLOWY electric purple 😍</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq29em</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1dq1qci</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitter topper can hide all the mistakes </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3zwemi9jf69d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1dq1gev</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newb question about process order with respect to cuticle cream, oil, and painting? </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dq1gev/newb_question_about_process_order_with_respect_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1dq0lhy</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Pride Mani!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nldtoer7769d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1dq04kn</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Love this combo but my camera is terrible</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5z9iiutd369d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1dpzgg7</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Getting Mario Kart vibes 🌈 🚗</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3hbtcoly59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1dpzczx</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>My go-to pride nail look 🌈</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fx4yatoux59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1dpz8nx</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Porcelain Nails ~ Lacquer Freehand </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpz8nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1dpys9g</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Sassy Sauce happy ending 💙💜</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpys9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1dpy7gg</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Floral Nails ✨️🌼</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpy7gg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1dpxvvj</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Bite Your Tongue 🗡️</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpxvvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1dpxi3y</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Eddie Sugar Daddy name change?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dpxi3y/eddie_sugar_daddy_name_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1dpxb6f</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Dark Eyes Blossom</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpxb6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1dpw56n</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Had to do a skittle for Pride Month. 🏳️‍🌈 Rare Cindy hand appearance!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpw56n</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1dpw3fb</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>IT CAME!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rperjz1t959d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1dpvj4c</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>What i asked , nails pink🥰</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou2yke5o559d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1dpvgs7</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Tried polka dots for the first time !!</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e82k74l7559d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1dpuo2w</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>My first mooncat order!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvrttbw9z49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1dpuk9t</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Can someone please help me find a dupe for Revlon Italian Leather?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpuk9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1dpt1lu</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smileys and rainbows </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lity86j4n49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1dpsrrb</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Hi all! I’m new to doing my own manicures at home. I had no clue how difficult chromes were to make look good!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb08ndzyk49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1dpsqfq</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Mojo Jojo</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpsqfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1dprpvl</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Aggressively Orange</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jac0l62oc49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1dprgyp</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>is this a good set ? first time getting a french manicure.</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dprgyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1dpqexc</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Debutante of my summer nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ssshz1h149d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1dppk10</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Pastel lemon recs?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dppk10/pastel_lemon_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1dpob8f</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Shellac peels off, WHY</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a14r6vig39d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1dpo0i4</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>KB Shimmer vs Chamaeleon Nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dpo0i4/kb_shimmer_vs_chamaeleon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1dpmlxm</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Issues with press ons</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dpmlxm/issues_with_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1dpm3mz</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I have big Orange Cat Energy, and I wasn't my turn with the brain cell, and I forgot to wear gloves when I waxed my legs. Is there a way to get all the wax off my nails, or is my poor manicure cooked?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dpm3mz/i_have_big_orange_cat_energy_and_i_wasnt_my_turn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1dpm0z4</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>:)</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpm0z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1dqbfq4</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Did courage the cowardly dog nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rilw6i32t89d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1dq94ik</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sz4flg4y389d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1dq8sir</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pooh bear XL press ons! (By me) </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqilx90i389d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1dq8okt</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beach Nails! (By me) </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw1on3pg289d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1dq86sn</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday set for the birthday girl (done by me) </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sva4hzyux79d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1dq249z</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Press ons or acrylic? ☺️</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dq249z</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1dq0e1x</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>♥️♣️♦️♠️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89bqlr3o569d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1dq0dri</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apkks6ql569d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1dpyu3j</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Nailed it! 💅</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihyqj9wyt59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1dpyoas</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>What do you think about the art of painting pictures on nails? I enjoy experimenting with various artistic styles. Do you have a favorite style? Comment below and I’ll give it a try! Thank you.</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/87u9r9cis59d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1dpy9z7</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Finished making these in one hour, kinda rushed but I like the result</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omhnafpup59d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1dpw6rx</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Palm trees pedi</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpw6rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1dpuzo8</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>First ever press ons!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l5oumyn159d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1dpt0ln</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smileys and rainbows - My first time using builder gel </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nmyhlswm49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1dps6o2</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Hi lovee 💌</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3idi6soeg49d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1dps5kt</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Chillet from Palworld! (Video link in description)</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dps5kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1dpq62s</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>I wanted to show off my hand painted flowers too!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuo6rjq5z39d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1dpq3tb</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Tips for keeping workplace clean</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dpq3tb/tips_for_keeping_workplace_clean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1dpntnj</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Lucky</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaufqdqva39d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1dpn6or</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Simply beautiful ✨</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dpn6or</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun 29 08:08:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_30.xlsx
+++ b/data/2024_06_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C981"/>
+  <dimension ref="A1:C1153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17110,6 +17110,2930 @@
         </is>
       </c>
     </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1dr66xt</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Help, my nails are extra long</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znzly2ekwg9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1dr5nyj</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Lucked out with finding 15 year old press on nails from a nearby pharmacy</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr5nyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1dr5js4</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>First time having this long nails.</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l24796nbog9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1dr2lrk</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Strawberry Gingham🍓</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr2lrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1dr46kf</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>SET I DID FOR PRIDE MONTH!!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr46kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1dr1kz4</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>My favorite set I’ve ever gotten 🥹</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr1kz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1dr11ok</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Anxious autistic and a skin picker. Need help and I want a pedicure. Tips?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dr11ok/anxious_autistic_and_a_skin_picker_need_help_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1dqy6aw</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Twilight nails by Gellraiser</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8nmk2guje9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1dqw5t7</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>I’m really down about my Gel polish allergy - please help</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqw5t7/im_really_down_about_my_gel_polish_allergy_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1dqv8un</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>How bad are these?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqv8un</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1dqs8tu</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>As much as I love these nails and the 3D art, I do not love the $100 price tag 😭</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zrq99mlw7d9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1dqprye</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Press ons glued to gel???</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhas0ah2pc9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1dqjv4k</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>baby boy nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqjv4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1dqinnz</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Real Nails Thanks to BIAB</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqinnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1dr534n</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Good color that goes with anything?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dr534n/good_color_that_goes_with_anything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1dqfp8d</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>About gel x (?)</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqfp8d/about_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1dqdvdj</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Engagement Nail Ideas?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqdvdj/engagement_nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1dr4t9z</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Pride nails 🌈</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cay5shqgfg9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1dr3nxq</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>A little neon chrome moment</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y58bsqn42g9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1dr34sj</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Yaya or nay?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr34sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1dr2owx</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>one of my favorite pride nail sets ☁️🌈☁️</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyzgbhuirf9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1dr2j37</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>pride tips🌈</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr2j37</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1dr2e41</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Flower Nails</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr2e41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1dr1bhr</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Gel-x Nail Inspos🥰❤️</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr1bhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1dr17gm</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Citrus nails I did on myself!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wd4numhfcf9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1dr1709</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When your nails perfectly match your shorts </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghsxcpxacf9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1dr0p0j</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr0p0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1dqytbv</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>✨Biweekly set✨</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqytbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1dqzzst</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do refills work for these 2 weeks ago ? Can I get them repainted with white French tips or would that be considered a full set? </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fccd0uvw0f9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1dqzyxz</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help choosing </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plqew64q0f9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1dqzqx3</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo has my heart✨ 🌈 </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqzqx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1dqzjnz</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little different than my typical nude 🌶️ 🚀 </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0f4mkwpwe9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1dqzjgq</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP- Weird dark spots on fresh gel pedicure?? </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yat5tlmnwe9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1dqzftw</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Just finished these babies🥰</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqzftw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1dqz616</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Double tip me please!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqz616</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1dqz24q</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>aura nails 🩷🔗</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqz24q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1dqz1bc</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>The result of my first pedicure in over a year. I feel so cute.</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqz1bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1dqz0b6</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with bridesmaid nail selection? </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amvp1nkkre9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1dqyq76</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>I love the color and they get so many compliments from strangers!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/git3z46zoe9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1dqykq5</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Happy Fourth of July 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfnzqhilne9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1dqyiin</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>First time trying press ons, rate em 1-10</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqyiin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1dqyda9</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>My recent gel x set</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5f02rinle9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1dqxuej</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I love this simple nail design. What do you think? 💅</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqxuej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1dqxael</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Birthday nails! Gel over my natural nails</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab24u9e8ce9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1dqx574</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecj68ug0be9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1dqx0aq</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first time designing my own  press-ons! how did i do ?? </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqx0aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1dqwyob</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>I can’t stop looking at them🪁💖…help?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqwyob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1dqwp8w</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Keep the almond or switch to coffin?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwdz4rnb7e9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1dqwnp4</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>my nails in paris 🥐🎀</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqwnp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1dqw9kf</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Did 4th of July nails. Do I hate them? Yup. Am I too lazy to change them? Also yup. Lol</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ef3gebm3e9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1dqw8cx</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>My tech did her thang today💅🏼🪻</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l91ddqb3e9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1dqw3oc</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Wedding Nail Trial 😍</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqw3oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1dqw1x9</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>used top coat instead of builder gel for full top extensions</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lhb2x1u1e9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1dqvy8n</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My favorite I’ve done for myself so far!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ya3ub4201e9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1dqvq43</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Gel Nails Virgin: Advice Needed</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oybhrt58zd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1dqvnxs</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>I got impatient....</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55tlo0bqyd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1dqvb9s</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>i love these</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ob3xolayvd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1dqvatv</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Aura nails for a bright summer vibe 💚💙</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqvatv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1dqv6a6</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>delicate flowers</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dk9n0xtud9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1dqv4d0</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>not the very first time, but still... what did i do wrong?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9sid4yytd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1dqr275</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Dry+flaky cuticles. What do I do?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jaklqkuyc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1dqufco</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>My chihuahua bites</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqufco/my_chihuahua_bites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1dquaat</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Tie Dye </t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dquaat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1dqu04r</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Recent nail sets have been fun ✨ structured manicures done with hard gel on my clients natural nails</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/igvnwubhld9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1dqt3cx</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Summer is here 🦩</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p0k3qeied9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1dqs8ah</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Should I just cut them and start over? (Natural nails. Gel Polish)</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqs8ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1dqs43x</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Fave set of press ons yet!</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqs43x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1dqrsiy</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Nailpaint Colour Dupe</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/C4QuOYsLke2/?igsh=Z29jdWJwdHVyNHZk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1dqrh56</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>I love them !!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkfvmukz1d9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1dqrcik</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Duck nails appreciation post🦆</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ysuhmt101d9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1dqrapc</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Did these on my cousin and I’m obsessed 🥹</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9qb3bjn0d9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1dqqxbs</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Subtle 4th of July Nails ⭐️</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87xvayntxc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1dqqsdf</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>For Charli</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqqsdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1dqq907</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Started getting my nails done recently and I’m in love!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w11qmwdksc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1dqq7um</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>yellow/pink nails</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qozfspodsc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1dqq18w</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>help! dont like my nails :(</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqq18w/help_dont_like_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1dqq141</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>golden hour didn’t do my two cateye claws justice</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqq141</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1dqphqk</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>4th of July</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/221h9ievmc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1dqlepe</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Would you date a guy with these nails</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tj7hs9csb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1dqmd6y</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Growing natural nails</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqmd6y/growing_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1dqoi9k</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>One of my favorite sets…</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkxxsbbhfc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1dqmwy8</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>How to stop gel from bubbling when wet?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqmwy8/how_to_stop_gel_from_bubbling_when_wet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1dqo9xc</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Chrome nails are my new favorite.</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guitiifpdc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1dqo1lf</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Did these on my client’s NATURAL nails!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si1xjaczbc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1dqnpy0</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>My press ons for this week! I adore pink and glitter</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efgpmlbj9c9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1dqnot7</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su1ix93b9c9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1dqnh44</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Short overlay for grey and lilac themed wedding</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqnh44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1dqnb9h</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Shaky start, but I'm really enjoying the self care of doing my own nails again after 20 yrs.</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqnb9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1dqn5yx</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>New gems!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4ivvnxg5c9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1dqmqp5</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>New nails 💅🏻🦋</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqmqp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1dqmnkt</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Critique me PLS</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqmnkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1dqmj2z</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Nail ideas for plum and teal dresses?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqmj2z/nail_ideas_for_plum_and_teal_dresses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1dqm6zk</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Nail strengthener?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqm6zk/nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1dqm3q4</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Gel Polish Lifting</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqm3q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1dqlr4u</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Pink Rose Nails</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch4ettsyub9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1dqlpqo</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is OPI Semi Permanent Nail Polish worth it? </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dqlpqo/is_opi_semi_permanent_nail_polish_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1dqlm1z</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>new nails🩵</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqlm1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1dqlgnx</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Painted some Boomer nails on my Boomer MIL</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5qjq8trsb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1dqldf4</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Today’s nails!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yu3tqyd2sb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1dqk793</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Nail colour with engagement ring</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqk793</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1dr5pui</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Gel to regular polish shade match</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr5pui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1dr50l7</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Chama-chama-chameleooooon🪁💖</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2r7f2vrthg9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1dr49zj</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Shade match gel to regular polish</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr49zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1dr3kaa</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Who is getting Baja Blasted this weekend?!</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr3kaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1dr1500</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>On W̶e̶d̶n̶e̶s̶d̶a̶y̶s̶ FRIDAYS we wear pink</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7zfzbkrbf9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1dr0kng</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Help finding this color? 💖</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvfjc0wb6f9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1dr0ila</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>My first Fancy Gloss order</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj7m5oqs5f9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1dr0bl4</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I broke a nail and now i dont know what to do with myself</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr0bl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1dr05oo</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>PPU Haul! Ethereal’s See You Space Cowboy</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr05oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1dqzxyf</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>serpent venom + rothko red 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rw8zgfah0f9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1dqzrfp</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Wearing BKL's Queen of Rot while I wait for my Elden Ring order to come in</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqzrfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1dqz5gn</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>UV/LED Top coats VS Regular top coats</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqz5gn/uvled_top_coats_vs_regular_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1dqyyb1</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginning my nail journey! </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zftb2t1re9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1dqyu3g</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Well I definitly don't need the new Mooncat collection</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqyu3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1dqy4yv</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Juicy Mango Jelly 🧡</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quw4aupjje9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1dqy3nx</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Blurring Base Coats</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqy3nx/blurring_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1dqwq9b</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>THIS. IS. CAELID!!</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqwq9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1dqw4ns</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>PSA: Cirque brushes compatible with Night Owl Lacquer!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb28y6mg2e9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1dqvv7y</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Pink sparkles for Janelle Monaé</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqvv7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1dqu5su</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>A Cancer season slam dunk 🦀🌔🌙🌊</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xd7x9yytmd9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1dqu3a5</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Bar Glitter Jelly Sandwich</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5xgofhbmd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1dqtij7</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bee's Knees Lacquer, Become the Art Yourself </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqtij7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1dqtfcd</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Ether Dragon is so versatile!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqtfcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1dqt199</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer - Reaper vs. Chaos</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzt8nx62ed9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1dqsidd</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Received my first LynB order yesterday! </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqsidd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1dqsdmh</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>ILNP flower child</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqsdmh/ilnp_flower_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1dqrtqz</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Summer of rose tinted glasses and shimmer blue skies</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymet84i54d9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1dqrpsn</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Millennia by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqrpsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1dqrme6</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Mooncat x PPG🩵🩷💚</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqrme6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1dqr31c</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>My nail guy CLEARED 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6dhzwl0zc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1dqq8zo</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>And iiiiIiiiieeeeiiii will always loooove yoooOOOou</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xo8y0ydmsc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1dqpk26</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>So shiny!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrsbtk6cnc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1dqp0nv</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Lazy gradient with jelly polish 💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqp0nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1dqonej</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Can I achieve this kind of look with regular lacquer instead of gel?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v7ds3ujgc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1dqoksx</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Excuse the terrible train photo, but this always reminds me of the sun glinting off a sandy beach and gives me maximum summer vibes!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bd9y2mgzfc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1dqobo2</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Blossom 🌸</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqobo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1dqn03h</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Just having a little fun 💅</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqn03h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1dqmqz3</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Ocean man, take me by the (polished) hand</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq9a9gbf2c9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1dqma8n</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I love a good chop</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqma8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1dqlhb9</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Pastel neons for Pride</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbzw1nmwsb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1dql60e</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Daveen’s Dreamer (LE)</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjqvjjqfqb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1dqkxv8</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Cosmic Polish - an Australian brand 😍</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/931x3xumob9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1dqkt3v</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blurple is my new favorite color! </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea09c12mnb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1dqko4o</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Rimmel Rapid Ruby does, in fact, match my ruby 🌹</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgwvpx9jmb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1dqjwtg</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Desperately looking for a color match to this dolls dress</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxn94nycgb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1dqjjat</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Different versions of Seche Vite with different ingredients</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqjjat/different_versions_of_seche_vite_with_different/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1dqjeep</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can never go wrong with a blue + gold shimmer </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsr28emvbb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1dqixa1</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Coronation limited batch</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dqixa1/coronation_limited_batch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1dqipzm</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Polish to match mood of depression with flecks of happiness</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqipzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1dqi4sy</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Cloud My Vision by Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqi4sy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1dr4ss5</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>She looks pretty from a distance~</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlcpsq0bfg9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1dr4of6</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Another unfinished set~!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5g6ih4wdg9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1dr326z</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Ocean vibes😍 but where exactly to?? 💅🌺 🌊🪸</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr326z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1dr2cw6</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Recommended products / brands</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dr2cw6/recommended_products_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1dr11xb</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Got a commission for Alice in Wonderland nails!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m4ivi2xaf9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1dqyh43</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>First press ons I've ever done</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqyh43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1dqy6l4</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Vacation nails! 🐚⭐️</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqy6l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1dqvvaj</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Hello, look at this cute design I made, elegant nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fll9savzd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1dqu9uf</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short nails </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/594lppiqnd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1dqsubq</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pop art nails with gems 💎 (by me) </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjmjpdukcd9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1dqsce6</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>School/Teacher Nail Art Inspo</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjk5aqnr8d9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1dqrvxw</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Pastel Pink, Donut Glaze, and Glitter!!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oawzomq65d9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1dqrpab</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>My nail girl is AAA-mazing 🥹</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqrpab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1dqrou5</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>What do you think of my almond-shaped nails?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmmbvx9o3d9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1dqq4wq</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>today it's my turn 🌈</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faoejw0qrc9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1dqmz2d</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Been practicing auras recently! Loving the green combo!💚</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqmz2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1dqmrch</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Swirly fun 💚🩶</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqmrch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1dqlwhi</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Marbled frenchies Pride version 🌈🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qst1xlb2wb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1dqlfql</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>This week has been V E R S A T I L E ✨💜</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqlfql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1dqktu5</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>French tips are my new go-to nail style!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr7vu43snb9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1dqghez</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I couldn’t get leopard print out of my head so i decided to try it out :&gt;</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqghez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1dqfn6n</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Pink and chrome</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dqfn6n</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun 30 08:08:03 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_30.xlsx
+++ b/data/2024_06_30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1153"/>
+  <dimension ref="A1:C1332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20034,6 +20034,3049 @@
         </is>
       </c>
     </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1drvp8b</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Watermelon nails</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20woy3b8rn9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1drvab5</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Apres/Gel X extensions. Nude base. Dots &amp; nazar 🧿</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gjtt2us6mn9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1drv0f4</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drv0f4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1drux58</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Gel-x nail art</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs0c1wylhn9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1druvj3</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Just me trying to recapture my youth😉</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1druvj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1drpla9</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>DIY on myself</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drpla9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1druocc</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>went to see a new nail tech🫀</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1druocc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1druhdk</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry🍓 Fields </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1druhdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1druhab</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Queen’s Crown</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1druhab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1druc3g</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>nails for a party 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1druc3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1drtusl</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Pretty green</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drtusl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1drsdxc</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>tried press ons for the first time !</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3k4mifuom9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1drsart</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drsart</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1drs3ab</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">. Which ones do you guys like better? :) </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drs3ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1drroce</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drroce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1drrfm3</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My cute nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsp7f6w4fm9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1drrafn</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Googly eyes 👀😍</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/016dh34ndm9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1drqdh1</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>⭐️Sun⭐️</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snlviisj4m9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1drqd19</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>New cat eye🩵💚</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drqd19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1drqcup</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Favorite Nails I’ve Had Thus Far. 🐮🐄🛸👽</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43rr7z3d4m9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1drq4n1</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Took y’alls advice..redid set!!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drq4n1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1drps3m</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>I’m in love 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drps3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1drprl7</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>What is with the wrinkling at the base of my nail, near the cuticle? Am i doing something wrong with my press ons?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij8g7tkeyl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1drp6lv</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Inspo Pic vs Reality (Inspo from @NailsXMina on Insta)</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drp6lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1drpe1n</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Daughter wanted 4th of July nails</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bafoeowsul9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1drp9ya</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte Green </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga1xmznqtl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1drdnbf</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>What do I do, help me asap please 😭</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uj4kj7s3j9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1drigu0</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Broke my nail with gel x 7 days before my wedding!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drigu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1drj0vl</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Stop gel x nails falling off</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yfpxlbvbk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1drosgu</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Saturday, nail day</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g18i25j4pl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1droocd</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>I did it.</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjgz6ll0ol9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1drofrg</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>glitchy nails (diy)</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drofrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1drobqn</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>My friend started to learn nail art not long ago. I asked her if she could draw Mohg and Morgott's Great Rune. I think she did a good job. There are two more of her artworks on the right.</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsj0wiorkl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1drjj70</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Inspo vs result, she killed it! Inspo was @meraki_nails_cardiff</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drjj70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1drkq3f</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Honeymoon nail inspo wanted!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drkq3f/honeymoon_nail_inspo_wanted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1drl353</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Custom printed nail stickers?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drl353/custom_printed_nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1drl9xb</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You all inspired me </t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akbvhb0luk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1drldos</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>how do i remove acrylics without acetone?! 😭</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w77zc45dvk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1drluui</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Longtime round gal gone square</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drluui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1drnrd1</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Qq vcs acharam dessa cor de esmalte? Ignorem o fundo da foto, não tinha outro melhor-</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbqmxz5ufl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1drn5x1</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Smoke or no smoke?💨🌚</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drn5x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1drmvr2</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>July 4th</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyje2owa8l9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1drmscj</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>My Dream Nails</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drmscj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1drmrfx</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Best nail shape for my hand?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plbra48a7l9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1drmc5b</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Nails by my bestie</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cowguf2l3l9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1drm81y</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>💅 + ✨ + 🌈 = 😊</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drm81y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1drm70w</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Should I soak them off?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfwp0zed2l9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1drm565</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nail Growth </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdvmy8by1l9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1drlpop</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Recommendations for D(M)V Nail Artists</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drlpop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1drlocq</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Is this still a trend?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dep6dusxxk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1drln8d</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Gel not curing on full cover tips?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drln8d/gel_not_curing_on_full_cover_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1drlkhu</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Christmas nails from.. well, Christmas.</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drlkhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1drliw6</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>🌸💛</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drliw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1drlimp</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Summer 🌞💚</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odec606nwk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1drl9vu</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I am a sucker for simple glitter manis ✨</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drl9vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1drkpg1</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Nude, Slight ombré Chrome</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipp3xv2tpk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1drkoem</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Nail tech ate</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64xab6rkpk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1drklt0</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>winter gems!!!😍</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8hq9zwyok9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1drkkzz</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>4th of July Nails</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drkkzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1drkk5s</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Bright pink nails for my summer vacay!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qbc73rlok9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1drkga1</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>I got my nails done professionally for the first time! I got almond shaped, baby blue color :)</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drkga1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1drkdji</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>How adorable are these😍</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drkdji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1drkau2</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this was a week growth of some chrome nails I had </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t5bay7fmk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1drk6qq</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Simple Almond Nail fill</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c40acm6hlk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1drj88z</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>First time getting stickers instead of a hand-painted design, and I think these might be my new favorites ❤️</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2p3k4qkdk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1drj6p4</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Help! Should I ditch the stamping?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3ztefd8dk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1drj64x</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Non gel nail polish dupe please! (Photos I took last year)</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drj64x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1drir7d</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>I’ve gotten nonstop compliments on these!</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70n3pimn9k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1dripa0</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Textured chrome set</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnvhswas8k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1driedk</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>What is up with this nail :( it’s not flat like my other ones and sits at a weird angle</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eurnz1ro6k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1dri8i3</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>im a sucker for nude nails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pq4pwx6e5k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1dri80x</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>The color change...</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dri80x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1dri7ag</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>mid-exam season nails</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x0usdx45k9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1dri6cp</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Press-ons + builder gel</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dri6cp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1dri5su</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>1st time trying 3D art</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plguj9ks4k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1dri1tb</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>new set i did on myself 🍊🧡🏵️</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dri1tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1dri13g</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">simple, but cute </t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dri13g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1drhwaa</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>First time with natural nails in over a year</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qezkwwl2k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1drhw2r</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>New nails who dis</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drhw2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1drhvw4</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>I posted here a few weeks ago asking which shape worked the best - coffin/square won!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jajwo94j2k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1drhu3r</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>New work half done</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drhu3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1drhnph</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>new gel set i did myself!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drhnph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1drhn58</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Wanted something simple and delicate 🌟</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drhn58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1drhm8t</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Color and bling!</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kspcn0e0k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1drdrpc</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>If you line up your nail with the indentation at the bottom of the nail polish, it will look like you have painted with it.</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drdrpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1drgvx8</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>1st time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drgvx8/1st_time_getting_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1drc882</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>I did these nails the night before a first date. Thirty minutes into it I ended up in the hospital.</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkwrvl32si9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1drc746</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Why pushy on gel and color?!</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drc746/why_pushy_on_gel_and_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1drh0ro</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Nothing stays on my nails (pls help)</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drh0ro/nothing_stays_on_my_nails_pls_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1drgexc</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Second try with Gel-X tips for my wife 😊</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z34dqyeqj9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1drgcul</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i really love these </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drgcul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1drgakq</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Neon is just 🤤</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v5reb4fpj9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1drg48s</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Blue temp polish</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drg48s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1drfvp9</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>I’ve started a nail technician degree.</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1drfvp9/ive_started_a_nail_technician_degree/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1drf5g8</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Do you like pink and White or ombre nails?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjrddti2gj9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1drf53i</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Back to my comfort zone</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drf53i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1drf4fp</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>My favorite nails so far💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drf4fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1drexb2</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Tried to match my new car</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xp4oq18ej9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1drepxt</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Where can I get?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drepxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1dremrf</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What all do I need to start gelx at home? </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dremrf/what_all_do_i_need_to_start_gelx_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1drwjus</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>looking to start doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drwjus/looking_to_start_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1drw00j</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>looking for a white creme polish with colorful flakies/glitter</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drw00j/looking_for_a_white_creme_polish_with_colorful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1drv4o5</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>White Speckle Topper?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fahcbu8kn9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1drsrth</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Def flooded the cuticle but not bad for my 1st ever DIY gel. </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/112bhrvwsm9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1drs1sy</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>180 or 240 grit sanding band for nail prep?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drs1sy/180_or_240_grit_sanding_band_for_nail_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1drryrx</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>🦒 Nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drryrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1drr4g0</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>🥪💜</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drr4g0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1drr236</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Is this shade too dark to still be considered a nude? And does it suit me, iyo? I love it 💅🏽🤎</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drr236</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1drqh1u</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect combo: Mooncat Moonicorn &amp; Mermaid Bait </t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drqh1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1drpv2t</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>🪻spring mani in the summer☀️</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drpv2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1drpt4b</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>ISO a dupe for Chanel Pirate</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drpt4b/iso_a_dupe_for_chanel_pirate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1drpd87</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>The little mermaid</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drpd87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1droyyz</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>IRL difference?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1droyyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1drokzk</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Emily De Molly’s “Futuristic Bliss” (June PPU) is so dang pretty 🥹</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/93rwrdj6nl9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1drok67</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I’m staring over. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qz9twqa0nl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1dro8lw</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Help! mustard dyed my nail</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xfmye42kl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1drnsbz</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Yet another skittle mani :)</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drnsbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1drnllu</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Shleee Polish review, June 2024</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drnllu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1drnkku</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Saturday at home self care</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rz662w5el9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1drncj3</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>I got Sour Apple Rings during last year’s PPU rewind and I’m not surprised that it’s coming back again 🍏</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bwy9fracl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1drmbmb</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Mooncat Forces of Evil❤️</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drmbmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1drlxwy</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Peachy Floral &amp; Gold Flake 🌸✨</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drlxwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1drlqld</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Has anyone tried the French nail stamper tool on short nails?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drlqld/has_anyone_tried_the_french_nail_stamper_tool_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1drlk36</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Packaging appreciation post (and the polishes too 😜)</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drlk36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1drl3em</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Telling myself we have House of Hades at home (OPI Chopstix and Stones)</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drl3em</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1drl1dx</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Does anyone want 10 boxes of Apres Gel-X nails?? I’m only asking the cost to ship them to you. All sealed boxes. The site I ordered these from sent the wrong order but let me keep the product they sent for free! I use mostly long or ultra long nails &amp; these are all medium or short.</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drl1dx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1drkv7j</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>LynB I Do Drag-On Thermal</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drkv7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1drku45</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>metal ball in top coat???</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itpuv7pvqk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1drketj</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Has anyone had success w/ a 10lb horseshoe for velvetized magnetics?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc3wg40dnk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1drk6fn</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Best brands at Sally Beauty?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drk6fn/best_brands_at_sally_beauty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1drjsyk</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Ohana Means Family - Painted Polish w/matte topper</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drjsyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1drjra3</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>ILNP flower child. Whimsical and magical owo</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drjra3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1drj984</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Non-binary Nails for Pride Flags for Pride!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drj984</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1driwlh</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Pls ignore my dry skin and painted on cuticles but 💜</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1driwlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1dricwg</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Peach jelly 🍑</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dricwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1drhsea</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Silicone mat</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drhsea/silicone_mat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1drhpfk</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Floored by Fluorescent</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drhpfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1drh8ox</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Swatch of Oddities for PPU Rewind!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drh8ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1drh3q3</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Flower Power</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/27-6-2024-CStiMDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1drgmku</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Looking for a good lotion/hand cream to keep in my purse</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drgmku/looking_for_a_good_lotionhand_cream_to_keep_in_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1drfqn8</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Felt like doing a lazy gradient for Pride Month. The sun really did not wanna cooperate with me.</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drfqn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1drfq43</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8j7b3qvkj9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1drfbs4</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>I looked down during my workout and...</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drfbs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1drf5ix</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Bill remains a stunner</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drf5ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1drex6s</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Butterfly wings! </t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aza3q997ej9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1dreqrc</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Where can I get?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dreqrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1drdyzq</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Mooncat Mercury in Retrograde</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ti8uc5f6j9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1drdn0o</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Torrent by BKL is my new favorite shade</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drdn0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1drce6f</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Arcana</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l4raxigti9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1drcaia</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>✨️💜Purple Check💜✨️</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drcaia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1drboj8</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you’re in a blue green mood but can’t decide. </t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imj7u3hani9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1drbe2v</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Polish Pickup Rewind 2024 Complete List!</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1drbe2v/polish_pickup_rewind_2024_complete_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1dr9t10</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Me looking at all the awesome Pride nails, unable to paint her own nails because of job interviews. </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.giphy.com/media/v1.Y2lkPTc5MGI3NjExbGFxbXJuYTdyY2Z3Z3g4M3lsMmgwN2ZxdjVrb3pwcWMydW5kdGR2cSZlcD12MV9pbnRlcm5hbF9naWZfYnlfaWQmY3Q9Zw/26gJyhYbxYREkYlNK/giphy.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1dr9mo9</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Nail prep for press on nails</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afjq9rt53i9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1dr9kdw</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Swatch request Clionadh Thermonuclear +  Singularity</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dr9kdw/swatch_request_clionadh_thermonuclear_singularity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1drw227</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Pastel rainbows!</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcklg5dsvn9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1drttx3</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oranges 💅 </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drttx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1drrz0v</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>friend did these for me</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnmjmrjkkm9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1drrs9m</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>The other day I did these and I was delighted with the color 😻 but I don't want to repeat myself, can you send me inspiration to do with green nails?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f944a6vnim9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1drq45p</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>A client commissioned Alice in Wonderland nails and I LOVE how they turned out 💕</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7rscpbx1m9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1drnafd</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Saint Seiya inspired press-on nails</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugvd6q7sbl9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1drmpjh</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Did my own nails and I’m kinda obsessed 🥹</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vitouost6l9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1drma9v</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Any substitutes for liquid latex?</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1drma9v/any_substitutes_for_liquid_latex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1drlvp1</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Mis nails aesthetic 🇦🇷</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y00kkknlzk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1drluiu</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>I love the color pink and glitter</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zybl0f62zk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1drklzz</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gitch effect nails </t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drklzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1drk9gr</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>gel nails I had from a month or so ago, this combo was so pretty, and this was a week growth</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y086beb4mk9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1drk15w</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>bratz</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drk15w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1drju15</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Today I chose daisies combined with a black base. I love them ❤️</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drju15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1drjeam</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Notd 🎀</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0lgktkxek9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1driec6</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>A set I've been working on- inspo came from part of an Alleycoolcatt set on Insta!</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doqs8vqo6k9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1dri0t8</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Figuring out how to nail art can be hard…</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dri0t8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1drhhg0</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Blue and Silver Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drhhg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1dre2vx</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Something about stilettos 😍</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dre2vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1drdbgz</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The perfect summer nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1drdbgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1draxle</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Aurora nailart inspirations</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1draxle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1dr8s05</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>got this cool pattern after patting eyeshadow on half dry base coat, and then topping with seche vite. i hope i can replicate it!!!</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oiwt9qikth9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1dr7z49</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Recreated the VIRAL Lily nails</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr7z49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1dr6hns</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Seeing Hamilton tonight- was only right to make my nails match the vibes!</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dr6hns</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>